<commit_message>
Feedback dimitri module 3 + klaarzetten bestanden lkr
</commit_message>
<xml_diff>
--- a/testMaartApril/contactgegevensLeerkrachten.xlsx
+++ b/testMaartApril/contactgegevensLeerkrachten.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
   <si>
     <t>Interesse hartslagmeter</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Bieke Sarens</t>
-  </si>
-  <si>
-    <t>jA</t>
   </si>
   <si>
     <t>Natacha Gesquière</t>
@@ -221,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +237,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -254,13 +257,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,8 +752,8 @@
       <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>50</v>
+      <c r="H10" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,7 +863,7 @@
         <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -867,13 +871,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>

</xml_diff>